<commit_message>
cleaned up urs export
</commit_message>
<xml_diff>
--- a/templates/старая_учетка_УРС.xlsx
+++ b/templates/старая_учетка_УРС.xlsx
@@ -62,11 +62,11 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="Огнедышащий воробей - Личное представление" guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" autoUpdate="1" mergeInterval="5" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1024" windowHeight="548" tabRatio="919" activeSheetId="8"/>
+    <customWorkbookView name="Учебный отдел - Личное представление" guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="729" activeSheetId="3"/>
+    <customWorkbookView name="Michael - Личное представление" guid="{B3126DA8-A41F-46B2-A2D2-24150549518C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="788" windowHeight="457" tabRatio="766" activeSheetId="8"/>
+    <customWorkbookView name="M@N - Личное представление" guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="832" activeSheetId="13"/>
     <customWorkbookView name="Admin - Личное представление" guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="767" tabRatio="919" activeSheetId="2"/>
-    <customWorkbookView name="M@N - Личное представление" guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="832" activeSheetId="13"/>
-    <customWorkbookView name="Michael - Личное представление" guid="{B3126DA8-A41F-46B2-A2D2-24150549518C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="788" windowHeight="457" tabRatio="766" activeSheetId="8"/>
-    <customWorkbookView name="Учебный отдел - Личное представление" guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="408" tabRatio="729" activeSheetId="3"/>
-    <customWorkbookView name="Огнедышащий воробей - Личное представление" guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" autoUpdate="1" mergeInterval="5" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1024" windowHeight="548" tabRatio="919" activeSheetId="8"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1772,7 +1772,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="295">
+  <cellXfs count="296">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2456,6 +2456,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2484,56 +2529,11 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2558,15 +2558,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2599,8 +2590,20 @@
     <xf numFmtId="0" fontId="18" fillId="26" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3044,697 +3047,697 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="249" t="s">
+      <c r="A1" s="264" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="250"/>
-      <c r="I1" s="250"/>
-      <c r="J1" s="250"/>
-      <c r="K1" s="250"/>
-      <c r="L1" s="250"/>
-      <c r="M1" s="250"/>
-      <c r="N1" s="250"/>
-      <c r="O1" s="250"/>
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="265"/>
+      <c r="F1" s="265"/>
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="265"/>
+      <c r="M1" s="265"/>
+      <c r="N1" s="265"/>
+      <c r="O1" s="265"/>
       <c r="P1" s="134"/>
     </row>
     <row r="2" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="250" t="s">
+      <c r="A2" s="265" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="250"/>
-      <c r="C2" s="250"/>
-      <c r="D2" s="250"/>
-      <c r="E2" s="250"/>
-      <c r="F2" s="250"/>
-      <c r="G2" s="250"/>
-      <c r="H2" s="250"/>
-      <c r="I2" s="250"/>
-      <c r="J2" s="250"/>
-      <c r="K2" s="250"/>
-      <c r="L2" s="250"/>
-      <c r="M2" s="250"/>
-      <c r="N2" s="250"/>
-      <c r="O2" s="250"/>
+      <c r="B2" s="265"/>
+      <c r="C2" s="265"/>
+      <c r="D2" s="265"/>
+      <c r="E2" s="265"/>
+      <c r="F2" s="265"/>
+      <c r="G2" s="265"/>
+      <c r="H2" s="265"/>
+      <c r="I2" s="265"/>
+      <c r="J2" s="265"/>
+      <c r="K2" s="265"/>
+      <c r="L2" s="265"/>
+      <c r="M2" s="265"/>
+      <c r="N2" s="265"/>
+      <c r="O2" s="265"/>
       <c r="P2" s="134"/>
     </row>
     <row r="3" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="251" t="s">
+      <c r="A3" s="266" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="251"/>
-      <c r="C3" s="251"/>
-      <c r="D3" s="251"/>
-      <c r="E3" s="251"/>
-      <c r="F3" s="251"/>
-      <c r="G3" s="251"/>
-      <c r="H3" s="251"/>
-      <c r="I3" s="251"/>
-      <c r="J3" s="251"/>
-      <c r="K3" s="251"/>
-      <c r="L3" s="251"/>
-      <c r="M3" s="251"/>
-      <c r="N3" s="251"/>
-      <c r="O3" s="251"/>
+      <c r="B3" s="266"/>
+      <c r="C3" s="266"/>
+      <c r="D3" s="266"/>
+      <c r="E3" s="266"/>
+      <c r="F3" s="266"/>
+      <c r="G3" s="266"/>
+      <c r="H3" s="266"/>
+      <c r="I3" s="266"/>
+      <c r="J3" s="266"/>
+      <c r="K3" s="266"/>
+      <c r="L3" s="266"/>
+      <c r="M3" s="266"/>
+      <c r="N3" s="266"/>
+      <c r="O3" s="266"/>
       <c r="P3" s="134"/>
     </row>
     <row r="4" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="252" t="s">
+      <c r="A4" s="267" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="252"/>
-      <c r="C4" s="252"/>
-      <c r="D4" s="252"/>
-      <c r="E4" s="252"/>
-      <c r="F4" s="252"/>
-      <c r="G4" s="252"/>
-      <c r="H4" s="252"/>
-      <c r="I4" s="252"/>
-      <c r="J4" s="252"/>
-      <c r="K4" s="252"/>
-      <c r="L4" s="252"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="252"/>
-      <c r="O4" s="252"/>
+      <c r="B4" s="267"/>
+      <c r="C4" s="267"/>
+      <c r="D4" s="267"/>
+      <c r="E4" s="267"/>
+      <c r="F4" s="267"/>
+      <c r="G4" s="267"/>
+      <c r="H4" s="267"/>
+      <c r="I4" s="267"/>
+      <c r="J4" s="267"/>
+      <c r="K4" s="267"/>
+      <c r="L4" s="267"/>
+      <c r="M4" s="267"/>
+      <c r="N4" s="267"/>
+      <c r="O4" s="267"/>
       <c r="P4" s="134"/>
     </row>
     <row r="5" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="253" t="s">
+      <c r="A5" s="268" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="253"/>
-      <c r="C5" s="253"/>
-      <c r="D5" s="253"/>
-      <c r="E5" s="253"/>
-      <c r="F5" s="253"/>
-      <c r="G5" s="253"/>
-      <c r="H5" s="253"/>
-      <c r="I5" s="253"/>
-      <c r="J5" s="253"/>
-      <c r="K5" s="253"/>
-      <c r="L5" s="253"/>
-      <c r="M5" s="253"/>
-      <c r="N5" s="253"/>
-      <c r="O5" s="253"/>
+      <c r="B5" s="268"/>
+      <c r="C5" s="268"/>
+      <c r="D5" s="268"/>
+      <c r="E5" s="268"/>
+      <c r="F5" s="268"/>
+      <c r="G5" s="268"/>
+      <c r="H5" s="268"/>
+      <c r="I5" s="268"/>
+      <c r="J5" s="268"/>
+      <c r="K5" s="268"/>
+      <c r="L5" s="268"/>
+      <c r="M5" s="268"/>
+      <c r="N5" s="268"/>
+      <c r="O5" s="268"/>
       <c r="P5" s="134"/>
     </row>
     <row r="6" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="247" t="s">
+      <c r="A6" s="262" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="247"/>
-      <c r="C6" s="247"/>
-      <c r="D6" s="247"/>
-      <c r="E6" s="247"/>
-      <c r="F6" s="247"/>
-      <c r="G6" s="247"/>
-      <c r="H6" s="247"/>
-      <c r="I6" s="247"/>
-      <c r="J6" s="247"/>
-      <c r="K6" s="247"/>
-      <c r="L6" s="247"/>
-      <c r="M6" s="247"/>
-      <c r="N6" s="247"/>
-      <c r="O6" s="247"/>
+      <c r="B6" s="262"/>
+      <c r="C6" s="262"/>
+      <c r="D6" s="262"/>
+      <c r="E6" s="262"/>
+      <c r="F6" s="262"/>
+      <c r="G6" s="262"/>
+      <c r="H6" s="262"/>
+      <c r="I6" s="262"/>
+      <c r="J6" s="262"/>
+      <c r="K6" s="262"/>
+      <c r="L6" s="262"/>
+      <c r="M6" s="262"/>
+      <c r="N6" s="262"/>
+      <c r="O6" s="262"/>
       <c r="P6" s="134"/>
     </row>
     <row r="7" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="254" t="s">
+      <c r="A7" s="269" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="255"/>
-      <c r="C7" s="255"/>
-      <c r="D7" s="255"/>
-      <c r="E7" s="255"/>
-      <c r="F7" s="255"/>
-      <c r="G7" s="255"/>
-      <c r="H7" s="255"/>
-      <c r="I7" s="255"/>
-      <c r="J7" s="255"/>
-      <c r="K7" s="255"/>
-      <c r="L7" s="255"/>
-      <c r="M7" s="255"/>
-      <c r="N7" s="255"/>
-      <c r="O7" s="255"/>
+      <c r="B7" s="270"/>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
+      <c r="E7" s="270"/>
+      <c r="F7" s="270"/>
+      <c r="G7" s="270"/>
+      <c r="H7" s="270"/>
+      <c r="I7" s="270"/>
+      <c r="J7" s="270"/>
+      <c r="K7" s="270"/>
+      <c r="L7" s="270"/>
+      <c r="M7" s="270"/>
+      <c r="N7" s="270"/>
+      <c r="O7" s="270"/>
       <c r="P7" s="134"/>
     </row>
     <row r="8" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="256" t="s">
+      <c r="A8" s="271" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="257"/>
-      <c r="C8" s="257"/>
-      <c r="D8" s="257"/>
-      <c r="E8" s="257"/>
-      <c r="F8" s="257"/>
-      <c r="G8" s="257"/>
-      <c r="H8" s="257"/>
-      <c r="I8" s="257"/>
-      <c r="J8" s="257"/>
-      <c r="K8" s="257"/>
-      <c r="L8" s="257"/>
-      <c r="M8" s="257"/>
-      <c r="N8" s="257"/>
-      <c r="O8" s="257"/>
+      <c r="B8" s="256"/>
+      <c r="C8" s="256"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
+      <c r="G8" s="256"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="256"/>
+      <c r="J8" s="256"/>
+      <c r="K8" s="256"/>
+      <c r="L8" s="256"/>
+      <c r="M8" s="256"/>
+      <c r="N8" s="256"/>
+      <c r="O8" s="256"/>
       <c r="P8" s="134"/>
     </row>
     <row r="9" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="258" t="s">
+      <c r="A9" s="272" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="259"/>
-      <c r="C9" s="259"/>
-      <c r="D9" s="259"/>
-      <c r="E9" s="259"/>
-      <c r="F9" s="259"/>
-      <c r="G9" s="259"/>
-      <c r="H9" s="259"/>
-      <c r="I9" s="259"/>
-      <c r="J9" s="259"/>
-      <c r="K9" s="259"/>
-      <c r="L9" s="259"/>
-      <c r="M9" s="259"/>
-      <c r="N9" s="259"/>
-      <c r="O9" s="259"/>
+      <c r="B9" s="273"/>
+      <c r="C9" s="273"/>
+      <c r="D9" s="273"/>
+      <c r="E9" s="273"/>
+      <c r="F9" s="273"/>
+      <c r="G9" s="273"/>
+      <c r="H9" s="273"/>
+      <c r="I9" s="273"/>
+      <c r="J9" s="273"/>
+      <c r="K9" s="273"/>
+      <c r="L9" s="273"/>
+      <c r="M9" s="273"/>
+      <c r="N9" s="273"/>
+      <c r="O9" s="273"/>
       <c r="P9" s="134"/>
     </row>
     <row r="10" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="248" t="s">
+      <c r="A10" s="263" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="248"/>
-      <c r="C10" s="248"/>
-      <c r="D10" s="248"/>
-      <c r="E10" s="248"/>
-      <c r="F10" s="248"/>
-      <c r="G10" s="248"/>
-      <c r="H10" s="248"/>
-      <c r="I10" s="248"/>
-      <c r="J10" s="248"/>
-      <c r="K10" s="248"/>
-      <c r="L10" s="248"/>
-      <c r="M10" s="248"/>
-      <c r="N10" s="248"/>
-      <c r="O10" s="248"/>
+      <c r="B10" s="263"/>
+      <c r="C10" s="263"/>
+      <c r="D10" s="263"/>
+      <c r="E10" s="263"/>
+      <c r="F10" s="263"/>
+      <c r="G10" s="263"/>
+      <c r="H10" s="263"/>
+      <c r="I10" s="263"/>
+      <c r="J10" s="263"/>
+      <c r="K10" s="263"/>
+      <c r="L10" s="263"/>
+      <c r="M10" s="263"/>
+      <c r="N10" s="263"/>
+      <c r="O10" s="263"/>
       <c r="P10" s="134"/>
     </row>
     <row r="11" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="269" t="s">
+      <c r="A11" s="251" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="269"/>
-      <c r="C11" s="269"/>
-      <c r="D11" s="269"/>
-      <c r="E11" s="269"/>
-      <c r="F11" s="269"/>
-      <c r="G11" s="269"/>
-      <c r="H11" s="269"/>
-      <c r="I11" s="269"/>
-      <c r="J11" s="269"/>
-      <c r="K11" s="269"/>
-      <c r="L11" s="269"/>
-      <c r="M11" s="269"/>
-      <c r="N11" s="269"/>
-      <c r="O11" s="269"/>
+      <c r="B11" s="251"/>
+      <c r="C11" s="251"/>
+      <c r="D11" s="251"/>
+      <c r="E11" s="251"/>
+      <c r="F11" s="251"/>
+      <c r="G11" s="251"/>
+      <c r="H11" s="251"/>
+      <c r="I11" s="251"/>
+      <c r="J11" s="251"/>
+      <c r="K11" s="251"/>
+      <c r="L11" s="251"/>
+      <c r="M11" s="251"/>
+      <c r="N11" s="251"/>
+      <c r="O11" s="251"/>
       <c r="P11" s="134"/>
     </row>
     <row r="12" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="270" t="s">
+      <c r="A12" s="252" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="271"/>
-      <c r="C12" s="271"/>
-      <c r="D12" s="271"/>
-      <c r="E12" s="271"/>
-      <c r="F12" s="271"/>
-      <c r="G12" s="271"/>
-      <c r="H12" s="271"/>
-      <c r="I12" s="271"/>
-      <c r="J12" s="271"/>
-      <c r="K12" s="271"/>
-      <c r="L12" s="271"/>
-      <c r="M12" s="271"/>
-      <c r="N12" s="271"/>
-      <c r="O12" s="271"/>
+      <c r="B12" s="253"/>
+      <c r="C12" s="253"/>
+      <c r="D12" s="253"/>
+      <c r="E12" s="253"/>
+      <c r="F12" s="253"/>
+      <c r="G12" s="253"/>
+      <c r="H12" s="253"/>
+      <c r="I12" s="253"/>
+      <c r="J12" s="253"/>
+      <c r="K12" s="253"/>
+      <c r="L12" s="253"/>
+      <c r="M12" s="253"/>
+      <c r="N12" s="253"/>
+      <c r="O12" s="253"/>
       <c r="P12" s="134"/>
     </row>
     <row r="13" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="271" t="s">
+      <c r="A13" s="253" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="271"/>
-      <c r="C13" s="271"/>
-      <c r="D13" s="271"/>
-      <c r="E13" s="271"/>
-      <c r="F13" s="271"/>
-      <c r="G13" s="271"/>
-      <c r="H13" s="271"/>
-      <c r="I13" s="271"/>
-      <c r="J13" s="271"/>
-      <c r="K13" s="271"/>
-      <c r="L13" s="271"/>
-      <c r="M13" s="271"/>
-      <c r="N13" s="271"/>
-      <c r="O13" s="271"/>
+      <c r="B13" s="253"/>
+      <c r="C13" s="253"/>
+      <c r="D13" s="253"/>
+      <c r="E13" s="253"/>
+      <c r="F13" s="253"/>
+      <c r="G13" s="253"/>
+      <c r="H13" s="253"/>
+      <c r="I13" s="253"/>
+      <c r="J13" s="253"/>
+      <c r="K13" s="253"/>
+      <c r="L13" s="253"/>
+      <c r="M13" s="253"/>
+      <c r="N13" s="253"/>
+      <c r="O13" s="253"/>
       <c r="P13" s="134"/>
     </row>
     <row r="14" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="271" t="s">
+      <c r="A14" s="253" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="271"/>
-      <c r="C14" s="271"/>
-      <c r="D14" s="271"/>
-      <c r="E14" s="271"/>
-      <c r="F14" s="271"/>
-      <c r="G14" s="271"/>
-      <c r="H14" s="271"/>
-      <c r="I14" s="271"/>
-      <c r="J14" s="271"/>
-      <c r="K14" s="271"/>
-      <c r="L14" s="271"/>
-      <c r="M14" s="271"/>
-      <c r="N14" s="271"/>
-      <c r="O14" s="271"/>
+      <c r="B14" s="253"/>
+      <c r="C14" s="253"/>
+      <c r="D14" s="253"/>
+      <c r="E14" s="253"/>
+      <c r="F14" s="253"/>
+      <c r="G14" s="253"/>
+      <c r="H14" s="253"/>
+      <c r="I14" s="253"/>
+      <c r="J14" s="253"/>
+      <c r="K14" s="253"/>
+      <c r="L14" s="253"/>
+      <c r="M14" s="253"/>
+      <c r="N14" s="253"/>
+      <c r="O14" s="253"/>
       <c r="P14" s="134"/>
     </row>
     <row r="15" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="271" t="s">
+      <c r="A15" s="253" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="271"/>
-      <c r="C15" s="271"/>
-      <c r="D15" s="271"/>
-      <c r="E15" s="271"/>
-      <c r="F15" s="271"/>
-      <c r="G15" s="271"/>
-      <c r="H15" s="271"/>
-      <c r="I15" s="271"/>
-      <c r="J15" s="271"/>
-      <c r="K15" s="271"/>
-      <c r="L15" s="271"/>
-      <c r="M15" s="271"/>
-      <c r="N15" s="271"/>
-      <c r="O15" s="271"/>
+      <c r="B15" s="253"/>
+      <c r="C15" s="253"/>
+      <c r="D15" s="253"/>
+      <c r="E15" s="253"/>
+      <c r="F15" s="253"/>
+      <c r="G15" s="253"/>
+      <c r="H15" s="253"/>
+      <c r="I15" s="253"/>
+      <c r="J15" s="253"/>
+      <c r="K15" s="253"/>
+      <c r="L15" s="253"/>
+      <c r="M15" s="253"/>
+      <c r="N15" s="253"/>
+      <c r="O15" s="253"/>
       <c r="P15" s="134"/>
     </row>
     <row r="16" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="271" t="s">
+      <c r="A16" s="253" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="271"/>
-      <c r="C16" s="271"/>
-      <c r="D16" s="271"/>
-      <c r="E16" s="271"/>
-      <c r="F16" s="271"/>
-      <c r="G16" s="271"/>
-      <c r="H16" s="271"/>
-      <c r="I16" s="271"/>
-      <c r="J16" s="271"/>
-      <c r="K16" s="271"/>
-      <c r="L16" s="271"/>
-      <c r="M16" s="271"/>
-      <c r="N16" s="271"/>
-      <c r="O16" s="271"/>
+      <c r="B16" s="253"/>
+      <c r="C16" s="253"/>
+      <c r="D16" s="253"/>
+      <c r="E16" s="253"/>
+      <c r="F16" s="253"/>
+      <c r="G16" s="253"/>
+      <c r="H16" s="253"/>
+      <c r="I16" s="253"/>
+      <c r="J16" s="253"/>
+      <c r="K16" s="253"/>
+      <c r="L16" s="253"/>
+      <c r="M16" s="253"/>
+      <c r="N16" s="253"/>
+      <c r="O16" s="253"/>
       <c r="P16" s="134"/>
     </row>
     <row r="17" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="271" t="s">
+      <c r="A17" s="253" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="271"/>
-      <c r="C17" s="271"/>
-      <c r="D17" s="271"/>
-      <c r="E17" s="271"/>
-      <c r="F17" s="271"/>
-      <c r="G17" s="271"/>
-      <c r="H17" s="271"/>
-      <c r="I17" s="271"/>
-      <c r="J17" s="271"/>
-      <c r="K17" s="271"/>
-      <c r="L17" s="271"/>
-      <c r="M17" s="271"/>
-      <c r="N17" s="271"/>
-      <c r="O17" s="271"/>
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="253"/>
+      <c r="J17" s="253"/>
+      <c r="K17" s="253"/>
+      <c r="L17" s="253"/>
+      <c r="M17" s="253"/>
+      <c r="N17" s="253"/>
+      <c r="O17" s="253"/>
       <c r="P17" s="134"/>
     </row>
     <row r="18" spans="1:16" s="136" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="272" t="s">
+      <c r="A18" s="247" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="273"/>
-      <c r="C18" s="273"/>
-      <c r="D18" s="273"/>
-      <c r="E18" s="273"/>
-      <c r="F18" s="273"/>
-      <c r="G18" s="273"/>
-      <c r="H18" s="273"/>
-      <c r="I18" s="273"/>
-      <c r="J18" s="273"/>
-      <c r="K18" s="273"/>
-      <c r="L18" s="273"/>
-      <c r="M18" s="273"/>
-      <c r="N18" s="273"/>
-      <c r="O18" s="273"/>
+      <c r="B18" s="248"/>
+      <c r="C18" s="248"/>
+      <c r="D18" s="248"/>
+      <c r="E18" s="248"/>
+      <c r="F18" s="248"/>
+      <c r="G18" s="248"/>
+      <c r="H18" s="248"/>
+      <c r="I18" s="248"/>
+      <c r="J18" s="248"/>
+      <c r="K18" s="248"/>
+      <c r="L18" s="248"/>
+      <c r="M18" s="248"/>
+      <c r="N18" s="248"/>
+      <c r="O18" s="248"/>
       <c r="P18" s="134"/>
     </row>
     <row r="19" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="263" t="s">
+      <c r="A19" s="249" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="263"/>
-      <c r="C19" s="263"/>
-      <c r="D19" s="263"/>
-      <c r="E19" s="263"/>
-      <c r="F19" s="263"/>
-      <c r="G19" s="263"/>
-      <c r="H19" s="263"/>
-      <c r="I19" s="263"/>
-      <c r="J19" s="263"/>
-      <c r="K19" s="263"/>
-      <c r="L19" s="263"/>
-      <c r="M19" s="263"/>
-      <c r="N19" s="263"/>
-      <c r="O19" s="263"/>
+      <c r="B19" s="249"/>
+      <c r="C19" s="249"/>
+      <c r="D19" s="249"/>
+      <c r="E19" s="249"/>
+      <c r="F19" s="249"/>
+      <c r="G19" s="249"/>
+      <c r="H19" s="249"/>
+      <c r="I19" s="249"/>
+      <c r="J19" s="249"/>
+      <c r="K19" s="249"/>
+      <c r="L19" s="249"/>
+      <c r="M19" s="249"/>
+      <c r="N19" s="249"/>
+      <c r="O19" s="249"/>
       <c r="P19" s="134"/>
     </row>
     <row r="20" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="263" t="s">
+      <c r="A20" s="249" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="263"/>
-      <c r="C20" s="263"/>
-      <c r="D20" s="263"/>
-      <c r="E20" s="263"/>
-      <c r="F20" s="263"/>
-      <c r="G20" s="263"/>
-      <c r="H20" s="263"/>
-      <c r="I20" s="263"/>
-      <c r="J20" s="263"/>
-      <c r="K20" s="263"/>
-      <c r="L20" s="263"/>
-      <c r="M20" s="263"/>
-      <c r="N20" s="263"/>
-      <c r="O20" s="263"/>
+      <c r="B20" s="249"/>
+      <c r="C20" s="249"/>
+      <c r="D20" s="249"/>
+      <c r="E20" s="249"/>
+      <c r="F20" s="249"/>
+      <c r="G20" s="249"/>
+      <c r="H20" s="249"/>
+      <c r="I20" s="249"/>
+      <c r="J20" s="249"/>
+      <c r="K20" s="249"/>
+      <c r="L20" s="249"/>
+      <c r="M20" s="249"/>
+      <c r="N20" s="249"/>
+      <c r="O20" s="249"/>
       <c r="P20" s="134"/>
     </row>
     <row r="21" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="263" t="s">
+      <c r="A21" s="249" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="263"/>
-      <c r="C21" s="263"/>
-      <c r="D21" s="263"/>
-      <c r="E21" s="263"/>
-      <c r="F21" s="263"/>
-      <c r="G21" s="263"/>
-      <c r="H21" s="263"/>
-      <c r="I21" s="263"/>
-      <c r="J21" s="263"/>
-      <c r="K21" s="263"/>
-      <c r="L21" s="263"/>
-      <c r="M21" s="263"/>
-      <c r="N21" s="263"/>
-      <c r="O21" s="263"/>
+      <c r="B21" s="249"/>
+      <c r="C21" s="249"/>
+      <c r="D21" s="249"/>
+      <c r="E21" s="249"/>
+      <c r="F21" s="249"/>
+      <c r="G21" s="249"/>
+      <c r="H21" s="249"/>
+      <c r="I21" s="249"/>
+      <c r="J21" s="249"/>
+      <c r="K21" s="249"/>
+      <c r="L21" s="249"/>
+      <c r="M21" s="249"/>
+      <c r="N21" s="249"/>
+      <c r="O21" s="249"/>
       <c r="P21" s="134"/>
     </row>
     <row r="22" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="263" t="s">
+      <c r="A22" s="249" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="263"/>
-      <c r="C22" s="263"/>
-      <c r="D22" s="263"/>
-      <c r="E22" s="263"/>
-      <c r="F22" s="263"/>
-      <c r="G22" s="263"/>
-      <c r="H22" s="263"/>
-      <c r="I22" s="263"/>
-      <c r="J22" s="263"/>
-      <c r="K22" s="263"/>
-      <c r="L22" s="263"/>
-      <c r="M22" s="263"/>
-      <c r="N22" s="263"/>
-      <c r="O22" s="263"/>
+      <c r="B22" s="249"/>
+      <c r="C22" s="249"/>
+      <c r="D22" s="249"/>
+      <c r="E22" s="249"/>
+      <c r="F22" s="249"/>
+      <c r="G22" s="249"/>
+      <c r="H22" s="249"/>
+      <c r="I22" s="249"/>
+      <c r="J22" s="249"/>
+      <c r="K22" s="249"/>
+      <c r="L22" s="249"/>
+      <c r="M22" s="249"/>
+      <c r="N22" s="249"/>
+      <c r="O22" s="249"/>
       <c r="P22" s="134"/>
     </row>
     <row r="23" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="261" t="s">
+      <c r="A23" s="255" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="262"/>
-      <c r="C23" s="262"/>
-      <c r="D23" s="262"/>
-      <c r="E23" s="262"/>
-      <c r="F23" s="262"/>
-      <c r="G23" s="262"/>
-      <c r="H23" s="262"/>
-      <c r="I23" s="262"/>
-      <c r="J23" s="262"/>
-      <c r="K23" s="262"/>
-      <c r="L23" s="262"/>
-      <c r="M23" s="262"/>
-      <c r="N23" s="262"/>
-      <c r="O23" s="262"/>
+      <c r="B23" s="250"/>
+      <c r="C23" s="250"/>
+      <c r="D23" s="250"/>
+      <c r="E23" s="250"/>
+      <c r="F23" s="250"/>
+      <c r="G23" s="250"/>
+      <c r="H23" s="250"/>
+      <c r="I23" s="250"/>
+      <c r="J23" s="250"/>
+      <c r="K23" s="250"/>
+      <c r="L23" s="250"/>
+      <c r="M23" s="250"/>
+      <c r="N23" s="250"/>
+      <c r="O23" s="250"/>
       <c r="P23" s="134"/>
     </row>
     <row r="24" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="262" t="s">
+      <c r="A24" s="250" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="262"/>
-      <c r="C24" s="262"/>
-      <c r="D24" s="262"/>
-      <c r="E24" s="262"/>
-      <c r="F24" s="262"/>
-      <c r="G24" s="262"/>
-      <c r="H24" s="262"/>
-      <c r="I24" s="262"/>
-      <c r="J24" s="262"/>
-      <c r="K24" s="262"/>
-      <c r="L24" s="262"/>
-      <c r="M24" s="262"/>
-      <c r="N24" s="262"/>
-      <c r="O24" s="262"/>
+      <c r="B24" s="250"/>
+      <c r="C24" s="250"/>
+      <c r="D24" s="250"/>
+      <c r="E24" s="250"/>
+      <c r="F24" s="250"/>
+      <c r="G24" s="250"/>
+      <c r="H24" s="250"/>
+      <c r="I24" s="250"/>
+      <c r="J24" s="250"/>
+      <c r="K24" s="250"/>
+      <c r="L24" s="250"/>
+      <c r="M24" s="250"/>
+      <c r="N24" s="250"/>
+      <c r="O24" s="250"/>
       <c r="P24" s="134"/>
     </row>
     <row r="25" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="262" t="s">
+      <c r="A25" s="250" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="262"/>
-      <c r="C25" s="262"/>
-      <c r="D25" s="262"/>
-      <c r="E25" s="262"/>
-      <c r="F25" s="262"/>
-      <c r="G25" s="262"/>
-      <c r="H25" s="262"/>
-      <c r="I25" s="262"/>
-      <c r="J25" s="262"/>
-      <c r="K25" s="262"/>
-      <c r="L25" s="262"/>
-      <c r="M25" s="262"/>
-      <c r="N25" s="262"/>
-      <c r="O25" s="262"/>
+      <c r="B25" s="250"/>
+      <c r="C25" s="250"/>
+      <c r="D25" s="250"/>
+      <c r="E25" s="250"/>
+      <c r="F25" s="250"/>
+      <c r="G25" s="250"/>
+      <c r="H25" s="250"/>
+      <c r="I25" s="250"/>
+      <c r="J25" s="250"/>
+      <c r="K25" s="250"/>
+      <c r="L25" s="250"/>
+      <c r="M25" s="250"/>
+      <c r="N25" s="250"/>
+      <c r="O25" s="250"/>
       <c r="P25" s="134"/>
     </row>
     <row r="26" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="262" t="s">
+      <c r="A26" s="250" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="262"/>
-      <c r="C26" s="262"/>
-      <c r="D26" s="262"/>
-      <c r="E26" s="262"/>
-      <c r="F26" s="262"/>
-      <c r="G26" s="262"/>
-      <c r="H26" s="262"/>
-      <c r="I26" s="262"/>
-      <c r="J26" s="262"/>
-      <c r="K26" s="262"/>
-      <c r="L26" s="262"/>
-      <c r="M26" s="262"/>
-      <c r="N26" s="262"/>
-      <c r="O26" s="262"/>
+      <c r="B26" s="250"/>
+      <c r="C26" s="250"/>
+      <c r="D26" s="250"/>
+      <c r="E26" s="250"/>
+      <c r="F26" s="250"/>
+      <c r="G26" s="250"/>
+      <c r="H26" s="250"/>
+      <c r="I26" s="250"/>
+      <c r="J26" s="250"/>
+      <c r="K26" s="250"/>
+      <c r="L26" s="250"/>
+      <c r="M26" s="250"/>
+      <c r="N26" s="250"/>
+      <c r="O26" s="250"/>
       <c r="P26" s="134"/>
     </row>
     <row r="27" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="262" t="s">
+      <c r="A27" s="250" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="262"/>
-      <c r="C27" s="262"/>
-      <c r="D27" s="262"/>
-      <c r="E27" s="262"/>
-      <c r="F27" s="262"/>
-      <c r="G27" s="262"/>
-      <c r="H27" s="262"/>
-      <c r="I27" s="262"/>
-      <c r="J27" s="262"/>
-      <c r="K27" s="262"/>
-      <c r="L27" s="262"/>
-      <c r="M27" s="262"/>
-      <c r="N27" s="262"/>
-      <c r="O27" s="262"/>
+      <c r="B27" s="250"/>
+      <c r="C27" s="250"/>
+      <c r="D27" s="250"/>
+      <c r="E27" s="250"/>
+      <c r="F27" s="250"/>
+      <c r="G27" s="250"/>
+      <c r="H27" s="250"/>
+      <c r="I27" s="250"/>
+      <c r="J27" s="250"/>
+      <c r="K27" s="250"/>
+      <c r="L27" s="250"/>
+      <c r="M27" s="250"/>
+      <c r="N27" s="250"/>
+      <c r="O27" s="250"/>
       <c r="P27" s="134"/>
     </row>
     <row r="28" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="257" t="s">
+      <c r="A28" s="256" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="257"/>
-      <c r="C28" s="257"/>
-      <c r="D28" s="257"/>
-      <c r="E28" s="257"/>
-      <c r="F28" s="257"/>
-      <c r="G28" s="257"/>
-      <c r="H28" s="257"/>
-      <c r="I28" s="257"/>
-      <c r="J28" s="257"/>
-      <c r="K28" s="257"/>
-      <c r="L28" s="257"/>
-      <c r="M28" s="257"/>
-      <c r="N28" s="257"/>
-      <c r="O28" s="257"/>
+      <c r="B28" s="256"/>
+      <c r="C28" s="256"/>
+      <c r="D28" s="256"/>
+      <c r="E28" s="256"/>
+      <c r="F28" s="256"/>
+      <c r="G28" s="256"/>
+      <c r="H28" s="256"/>
+      <c r="I28" s="256"/>
+      <c r="J28" s="256"/>
+      <c r="K28" s="256"/>
+      <c r="L28" s="256"/>
+      <c r="M28" s="256"/>
+      <c r="N28" s="256"/>
+      <c r="O28" s="256"/>
       <c r="P28" s="134"/>
     </row>
     <row r="29" spans="1:16" s="174" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="265" t="s">
+      <c r="A29" s="258" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="265"/>
-      <c r="C29" s="265"/>
-      <c r="D29" s="265"/>
-      <c r="E29" s="265"/>
-      <c r="F29" s="265"/>
-      <c r="G29" s="265"/>
-      <c r="H29" s="265"/>
-      <c r="I29" s="265"/>
-      <c r="J29" s="265"/>
-      <c r="K29" s="265"/>
-      <c r="L29" s="265"/>
-      <c r="M29" s="265"/>
-      <c r="N29" s="265"/>
-      <c r="O29" s="265"/>
+      <c r="B29" s="258"/>
+      <c r="C29" s="258"/>
+      <c r="D29" s="258"/>
+      <c r="E29" s="258"/>
+      <c r="F29" s="258"/>
+      <c r="G29" s="258"/>
+      <c r="H29" s="258"/>
+      <c r="I29" s="258"/>
+      <c r="J29" s="258"/>
+      <c r="K29" s="258"/>
+      <c r="L29" s="258"/>
+      <c r="M29" s="258"/>
+      <c r="N29" s="258"/>
+      <c r="O29" s="258"/>
     </row>
     <row r="30" spans="1:16" s="174" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="266" t="s">
+      <c r="A30" s="259" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="266"/>
-      <c r="C30" s="266"/>
-      <c r="D30" s="266"/>
-      <c r="E30" s="266"/>
-      <c r="F30" s="266"/>
-      <c r="G30" s="266"/>
-      <c r="H30" s="266"/>
-      <c r="I30" s="266"/>
-      <c r="J30" s="266"/>
-      <c r="K30" s="266"/>
-      <c r="L30" s="266"/>
-      <c r="M30" s="266"/>
-      <c r="N30" s="266"/>
-      <c r="O30" s="266"/>
+      <c r="B30" s="259"/>
+      <c r="C30" s="259"/>
+      <c r="D30" s="259"/>
+      <c r="E30" s="259"/>
+      <c r="F30" s="259"/>
+      <c r="G30" s="259"/>
+      <c r="H30" s="259"/>
+      <c r="I30" s="259"/>
+      <c r="J30" s="259"/>
+      <c r="K30" s="259"/>
+      <c r="L30" s="259"/>
+      <c r="M30" s="259"/>
+      <c r="N30" s="259"/>
+      <c r="O30" s="259"/>
     </row>
     <row r="31" spans="1:16" s="174" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="267" t="s">
+      <c r="A31" s="260" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="267"/>
-      <c r="C31" s="267"/>
-      <c r="D31" s="267"/>
-      <c r="E31" s="267"/>
-      <c r="F31" s="267"/>
-      <c r="G31" s="267"/>
-      <c r="H31" s="267"/>
-      <c r="I31" s="267"/>
-      <c r="J31" s="267"/>
-      <c r="K31" s="267"/>
-      <c r="L31" s="267"/>
-      <c r="M31" s="267"/>
-      <c r="N31" s="267"/>
-      <c r="O31" s="267"/>
+      <c r="B31" s="260"/>
+      <c r="C31" s="260"/>
+      <c r="D31" s="260"/>
+      <c r="E31" s="260"/>
+      <c r="F31" s="260"/>
+      <c r="G31" s="260"/>
+      <c r="H31" s="260"/>
+      <c r="I31" s="260"/>
+      <c r="J31" s="260"/>
+      <c r="K31" s="260"/>
+      <c r="L31" s="260"/>
+      <c r="M31" s="260"/>
+      <c r="N31" s="260"/>
+      <c r="O31" s="260"/>
     </row>
     <row r="32" spans="1:16" s="174" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="266" t="s">
+      <c r="A32" s="259" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="266"/>
-      <c r="C32" s="266"/>
-      <c r="D32" s="266"/>
-      <c r="E32" s="266"/>
-      <c r="F32" s="266"/>
-      <c r="G32" s="266"/>
-      <c r="H32" s="266"/>
-      <c r="I32" s="266"/>
-      <c r="J32" s="266"/>
-      <c r="K32" s="266"/>
-      <c r="L32" s="266"/>
-      <c r="M32" s="266"/>
-      <c r="N32" s="266"/>
-      <c r="O32" s="266"/>
+      <c r="B32" s="259"/>
+      <c r="C32" s="259"/>
+      <c r="D32" s="259"/>
+      <c r="E32" s="259"/>
+      <c r="F32" s="259"/>
+      <c r="G32" s="259"/>
+      <c r="H32" s="259"/>
+      <c r="I32" s="259"/>
+      <c r="J32" s="259"/>
+      <c r="K32" s="259"/>
+      <c r="L32" s="259"/>
+      <c r="M32" s="259"/>
+      <c r="N32" s="259"/>
+      <c r="O32" s="259"/>
     </row>
     <row r="33" spans="1:16" s="174" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="268" t="s">
+      <c r="A33" s="261" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="268"/>
-      <c r="C33" s="268"/>
-      <c r="D33" s="268"/>
-      <c r="E33" s="268"/>
-      <c r="F33" s="268"/>
-      <c r="G33" s="268"/>
-      <c r="H33" s="268"/>
-      <c r="I33" s="268"/>
-      <c r="J33" s="268"/>
-      <c r="K33" s="268"/>
-      <c r="L33" s="268"/>
-      <c r="M33" s="268"/>
-      <c r="N33" s="268"/>
-      <c r="O33" s="268"/>
+      <c r="B33" s="261"/>
+      <c r="C33" s="261"/>
+      <c r="D33" s="261"/>
+      <c r="E33" s="261"/>
+      <c r="F33" s="261"/>
+      <c r="G33" s="261"/>
+      <c r="H33" s="261"/>
+      <c r="I33" s="261"/>
+      <c r="J33" s="261"/>
+      <c r="K33" s="261"/>
+      <c r="L33" s="261"/>
+      <c r="M33" s="261"/>
+      <c r="N33" s="261"/>
+      <c r="O33" s="261"/>
     </row>
     <row r="34" spans="1:16" s="174" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="264" t="s">
+      <c r="A34" s="257" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="264"/>
-      <c r="C34" s="264"/>
-      <c r="D34" s="264"/>
-      <c r="E34" s="264"/>
-      <c r="F34" s="264"/>
-      <c r="G34" s="264"/>
-      <c r="H34" s="264"/>
-      <c r="I34" s="264"/>
-      <c r="J34" s="264"/>
-      <c r="K34" s="264"/>
-      <c r="L34" s="264"/>
-      <c r="M34" s="264"/>
-      <c r="N34" s="264"/>
-      <c r="O34" s="264"/>
+      <c r="B34" s="257"/>
+      <c r="C34" s="257"/>
+      <c r="D34" s="257"/>
+      <c r="E34" s="257"/>
+      <c r="F34" s="257"/>
+      <c r="G34" s="257"/>
+      <c r="H34" s="257"/>
+      <c r="I34" s="257"/>
+      <c r="J34" s="257"/>
+      <c r="K34" s="257"/>
+      <c r="L34" s="257"/>
+      <c r="M34" s="257"/>
+      <c r="N34" s="257"/>
+      <c r="O34" s="257"/>
     </row>
     <row r="35" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="260" t="s">
+      <c r="A35" s="254" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="260"/>
-      <c r="C35" s="260"/>
-      <c r="D35" s="260"/>
-      <c r="E35" s="260"/>
-      <c r="F35" s="260"/>
-      <c r="G35" s="260"/>
-      <c r="H35" s="260"/>
-      <c r="I35" s="260"/>
-      <c r="J35" s="260"/>
-      <c r="K35" s="260"/>
-      <c r="L35" s="260"/>
-      <c r="M35" s="260"/>
-      <c r="N35" s="260"/>
-      <c r="O35" s="260"/>
+      <c r="B35" s="254"/>
+      <c r="C35" s="254"/>
+      <c r="D35" s="254"/>
+      <c r="E35" s="254"/>
+      <c r="F35" s="254"/>
+      <c r="G35" s="254"/>
+      <c r="H35" s="254"/>
+      <c r="I35" s="254"/>
+      <c r="J35" s="254"/>
+      <c r="K35" s="254"/>
+      <c r="L35" s="254"/>
+      <c r="M35" s="254"/>
+      <c r="N35" s="254"/>
+      <c r="O35" s="254"/>
       <c r="P35" s="134"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
@@ -3775,15 +3778,15 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}">
-      <pane xSplit="15" ySplit="35" topLeftCell="P126" activePane="bottomRight" state="frozen"/>
+    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}">
+      <pane xSplit="15" ySplit="33" topLeftCell="P126" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="B131" sqref="B131"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}">
-      <pane xSplit="15" ySplit="33" topLeftCell="P126" activePane="bottomRight" state="frozen"/>
+    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}">
+      <pane xSplit="15" ySplit="35" topLeftCell="P126" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="B131" sqref="B131"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3791,18 +3794,16 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="35">
-    <mergeCell ref="A18:O18"/>
-    <mergeCell ref="A19:O19"/>
-    <mergeCell ref="A20:O20"/>
-    <mergeCell ref="A26:O26"/>
-    <mergeCell ref="A24:O24"/>
-    <mergeCell ref="A11:O11"/>
-    <mergeCell ref="A12:O12"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A17:O17"/>
-    <mergeCell ref="A15:O15"/>
-    <mergeCell ref="A16:O16"/>
+    <mergeCell ref="A6:O6"/>
+    <mergeCell ref="A10:O10"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A5:O5"/>
+    <mergeCell ref="A7:O7"/>
+    <mergeCell ref="A8:O8"/>
+    <mergeCell ref="A9:O9"/>
     <mergeCell ref="A35:O35"/>
     <mergeCell ref="A23:O23"/>
     <mergeCell ref="A27:O27"/>
@@ -3816,16 +3817,18 @@
     <mergeCell ref="A31:O31"/>
     <mergeCell ref="A32:O32"/>
     <mergeCell ref="A33:O33"/>
-    <mergeCell ref="A6:O6"/>
-    <mergeCell ref="A10:O10"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A5:O5"/>
-    <mergeCell ref="A7:O7"/>
-    <mergeCell ref="A8:O8"/>
-    <mergeCell ref="A9:O9"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="A12:O12"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="A17:O17"/>
+    <mergeCell ref="A15:O15"/>
+    <mergeCell ref="A16:O16"/>
+    <mergeCell ref="A18:O18"/>
+    <mergeCell ref="A19:O19"/>
+    <mergeCell ref="A20:O20"/>
+    <mergeCell ref="A26:O26"/>
+    <mergeCell ref="A24:O24"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3845,7 +3848,7 @@
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q79" sqref="Q79"/>
-      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
+      <selection pane="bottomLeft" activeCell="AB143" sqref="AB143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -3900,13 +3903,13 @@
       <c r="K1" s="211" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="120" t="s">
+      <c r="L1" s="295" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="120" t="s">
+      <c r="M1" s="295" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="120" t="s">
+      <c r="N1" s="295" t="s">
         <v>37</v>
       </c>
       <c r="O1" s="120" t="s">
@@ -3922,7 +3925,7 @@
         <v>82</v>
       </c>
       <c r="S1" s="120" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="T1" s="120" t="s">
         <v>85</v>
@@ -16737,7 +16740,7 @@
         <v>82</v>
       </c>
       <c r="S143" s="220" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="T143" s="220" t="s">
         <v>85</v>
@@ -17472,7 +17475,6 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" selectLockedCells="1" autoFilter="0"/>
-  <autoFilter ref="C3:D149"/>
   <sortState ref="C4:O136">
     <sortCondition ref="C4:C136"/>
     <sortCondition ref="E4:E136" customList="полковник,подполковник,майор,капитан,ст. лейтенант,лейтенант,ст. прапорщик,прапорщик,ст. сержант,сержант,мл. сержант,ефрейтор,рядовой"/>
@@ -17566,100 +17568,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:100" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="283" t="s">
+      <c r="A1" s="280" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="283"/>
-      <c r="C1" s="283"/>
-      <c r="D1" s="283"/>
-      <c r="E1" s="283"/>
-      <c r="F1" s="283"/>
-      <c r="G1" s="283"/>
-      <c r="H1" s="283"/>
-      <c r="I1" s="283"/>
-      <c r="J1" s="283"/>
-      <c r="K1" s="283"/>
-      <c r="L1" s="283"/>
-      <c r="M1" s="283"/>
-      <c r="N1" s="283"/>
-      <c r="O1" s="283"/>
-      <c r="P1" s="283"/>
-      <c r="Q1" s="283"/>
-      <c r="R1" s="283"/>
-      <c r="S1" s="283"/>
-      <c r="T1" s="283"/>
-      <c r="U1" s="283"/>
-      <c r="V1" s="283"/>
-      <c r="W1" s="283"/>
-      <c r="X1" s="283"/>
-      <c r="Y1" s="283"/>
-      <c r="Z1" s="283"/>
-      <c r="AA1" s="283"/>
-      <c r="AB1" s="283"/>
-      <c r="AC1" s="283"/>
-      <c r="AD1" s="283"/>
-      <c r="AE1" s="283"/>
-      <c r="AF1" s="283"/>
-      <c r="AG1" s="283"/>
-      <c r="AH1" s="283"/>
-      <c r="AI1" s="283"/>
-      <c r="AJ1" s="283"/>
-      <c r="AK1" s="283"/>
-      <c r="AL1" s="283"/>
-      <c r="AM1" s="283"/>
-      <c r="AN1" s="283"/>
-      <c r="AO1" s="283"/>
-      <c r="AP1" s="283"/>
-      <c r="AQ1" s="283"/>
-      <c r="AR1" s="283"/>
-      <c r="AS1" s="283"/>
-      <c r="AT1" s="283"/>
-      <c r="AU1" s="283"/>
-      <c r="AV1" s="283"/>
-      <c r="AW1" s="283"/>
-      <c r="AX1" s="283"/>
-      <c r="AY1" s="283"/>
-      <c r="AZ1" s="283"/>
-      <c r="BA1" s="283"/>
-      <c r="BB1" s="283"/>
-      <c r="BC1" s="283"/>
-      <c r="BD1" s="283"/>
-      <c r="BE1" s="283"/>
-      <c r="BF1" s="283"/>
-      <c r="BG1" s="283"/>
-      <c r="BH1" s="283"/>
-      <c r="BI1" s="283"/>
-      <c r="BJ1" s="283"/>
-      <c r="BK1" s="283"/>
-      <c r="BL1" s="283"/>
-      <c r="BM1" s="283"/>
-      <c r="BN1" s="283"/>
-      <c r="BO1" s="283"/>
-      <c r="BP1" s="283"/>
-      <c r="BQ1" s="283"/>
-      <c r="BR1" s="283"/>
-      <c r="BS1" s="283"/>
-      <c r="BT1" s="283"/>
-      <c r="BU1" s="283"/>
-      <c r="BV1" s="283"/>
-      <c r="BW1" s="283"/>
-      <c r="BX1" s="283"/>
-      <c r="BY1" s="283"/>
-      <c r="BZ1" s="283"/>
-      <c r="CA1" s="283"/>
-      <c r="CB1" s="283"/>
-      <c r="CC1" s="283"/>
-      <c r="CD1" s="283"/>
-      <c r="CE1" s="283"/>
-      <c r="CF1" s="283"/>
-      <c r="CG1" s="283"/>
-      <c r="CH1" s="283"/>
-      <c r="CI1" s="283"/>
-      <c r="CJ1" s="283"/>
-      <c r="CK1" s="283"/>
-      <c r="CL1" s="283"/>
-      <c r="CM1" s="283"/>
-      <c r="CN1" s="283"/>
+      <c r="B1" s="280"/>
+      <c r="C1" s="280"/>
+      <c r="D1" s="280"/>
+      <c r="E1" s="280"/>
+      <c r="F1" s="280"/>
+      <c r="G1" s="280"/>
+      <c r="H1" s="280"/>
+      <c r="I1" s="280"/>
+      <c r="J1" s="280"/>
+      <c r="K1" s="280"/>
+      <c r="L1" s="280"/>
+      <c r="M1" s="280"/>
+      <c r="N1" s="280"/>
+      <c r="O1" s="280"/>
+      <c r="P1" s="280"/>
+      <c r="Q1" s="280"/>
+      <c r="R1" s="280"/>
+      <c r="S1" s="280"/>
+      <c r="T1" s="280"/>
+      <c r="U1" s="280"/>
+      <c r="V1" s="280"/>
+      <c r="W1" s="280"/>
+      <c r="X1" s="280"/>
+      <c r="Y1" s="280"/>
+      <c r="Z1" s="280"/>
+      <c r="AA1" s="280"/>
+      <c r="AB1" s="280"/>
+      <c r="AC1" s="280"/>
+      <c r="AD1" s="280"/>
+      <c r="AE1" s="280"/>
+      <c r="AF1" s="280"/>
+      <c r="AG1" s="280"/>
+      <c r="AH1" s="280"/>
+      <c r="AI1" s="280"/>
+      <c r="AJ1" s="280"/>
+      <c r="AK1" s="280"/>
+      <c r="AL1" s="280"/>
+      <c r="AM1" s="280"/>
+      <c r="AN1" s="280"/>
+      <c r="AO1" s="280"/>
+      <c r="AP1" s="280"/>
+      <c r="AQ1" s="280"/>
+      <c r="AR1" s="280"/>
+      <c r="AS1" s="280"/>
+      <c r="AT1" s="280"/>
+      <c r="AU1" s="280"/>
+      <c r="AV1" s="280"/>
+      <c r="AW1" s="280"/>
+      <c r="AX1" s="280"/>
+      <c r="AY1" s="280"/>
+      <c r="AZ1" s="280"/>
+      <c r="BA1" s="280"/>
+      <c r="BB1" s="280"/>
+      <c r="BC1" s="280"/>
+      <c r="BD1" s="280"/>
+      <c r="BE1" s="280"/>
+      <c r="BF1" s="280"/>
+      <c r="BG1" s="280"/>
+      <c r="BH1" s="280"/>
+      <c r="BI1" s="280"/>
+      <c r="BJ1" s="280"/>
+      <c r="BK1" s="280"/>
+      <c r="BL1" s="280"/>
+      <c r="BM1" s="280"/>
+      <c r="BN1" s="280"/>
+      <c r="BO1" s="280"/>
+      <c r="BP1" s="280"/>
+      <c r="BQ1" s="280"/>
+      <c r="BR1" s="280"/>
+      <c r="BS1" s="280"/>
+      <c r="BT1" s="280"/>
+      <c r="BU1" s="280"/>
+      <c r="BV1" s="280"/>
+      <c r="BW1" s="280"/>
+      <c r="BX1" s="280"/>
+      <c r="BY1" s="280"/>
+      <c r="BZ1" s="280"/>
+      <c r="CA1" s="280"/>
+      <c r="CB1" s="280"/>
+      <c r="CC1" s="280"/>
+      <c r="CD1" s="280"/>
+      <c r="CE1" s="280"/>
+      <c r="CF1" s="280"/>
+      <c r="CG1" s="280"/>
+      <c r="CH1" s="280"/>
+      <c r="CI1" s="280"/>
+      <c r="CJ1" s="280"/>
+      <c r="CK1" s="280"/>
+      <c r="CL1" s="280"/>
+      <c r="CM1" s="280"/>
+      <c r="CN1" s="280"/>
       <c r="CP1" s="139"/>
       <c r="CQ1" s="139"/>
       <c r="CR1" s="139"/>
@@ -17669,102 +17671,102 @@
       <c r="CV1" s="139"/>
     </row>
     <row r="2" spans="1:100" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="289" t="s">
+      <c r="A2" s="286" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="291" t="s">
+      <c r="B2" s="288" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="286"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="287"/>
-      <c r="F2" s="287"/>
-      <c r="G2" s="287"/>
-      <c r="H2" s="287"/>
-      <c r="I2" s="287"/>
-      <c r="J2" s="287"/>
-      <c r="K2" s="287"/>
-      <c r="L2" s="287"/>
-      <c r="M2" s="287"/>
-      <c r="N2" s="287"/>
-      <c r="O2" s="287"/>
-      <c r="P2" s="287"/>
-      <c r="Q2" s="287"/>
-      <c r="R2" s="287"/>
-      <c r="S2" s="287"/>
-      <c r="T2" s="287"/>
-      <c r="U2" s="287"/>
-      <c r="V2" s="287"/>
-      <c r="W2" s="287"/>
-      <c r="X2" s="287"/>
-      <c r="Y2" s="287"/>
-      <c r="Z2" s="287"/>
-      <c r="AA2" s="287"/>
-      <c r="AB2" s="287"/>
-      <c r="AC2" s="287"/>
-      <c r="AD2" s="287"/>
-      <c r="AE2" s="287"/>
-      <c r="AF2" s="287"/>
-      <c r="AG2" s="287"/>
-      <c r="AH2" s="287"/>
-      <c r="AI2" s="287"/>
-      <c r="AJ2" s="287"/>
-      <c r="AK2" s="287"/>
-      <c r="AL2" s="287"/>
-      <c r="AM2" s="287"/>
-      <c r="AN2" s="287"/>
-      <c r="AO2" s="287"/>
-      <c r="AP2" s="287"/>
-      <c r="AQ2" s="287"/>
-      <c r="AR2" s="287"/>
-      <c r="AS2" s="287"/>
-      <c r="AT2" s="287"/>
-      <c r="AU2" s="287"/>
-      <c r="AV2" s="287"/>
-      <c r="AW2" s="287"/>
-      <c r="AX2" s="287"/>
-      <c r="AY2" s="287"/>
-      <c r="AZ2" s="287"/>
-      <c r="BA2" s="287"/>
-      <c r="BB2" s="287"/>
-      <c r="BC2" s="287"/>
-      <c r="BD2" s="287"/>
-      <c r="BE2" s="287"/>
-      <c r="BF2" s="287"/>
-      <c r="BG2" s="287"/>
-      <c r="BH2" s="287"/>
-      <c r="BI2" s="287"/>
-      <c r="BJ2" s="287"/>
-      <c r="BK2" s="287"/>
-      <c r="BL2" s="287"/>
-      <c r="BM2" s="287"/>
-      <c r="BN2" s="287"/>
-      <c r="BO2" s="287"/>
-      <c r="BP2" s="287"/>
-      <c r="BQ2" s="287"/>
-      <c r="BR2" s="287"/>
-      <c r="BS2" s="287"/>
-      <c r="BT2" s="287"/>
-      <c r="BU2" s="287"/>
-      <c r="BV2" s="287"/>
-      <c r="BW2" s="287"/>
-      <c r="BX2" s="287"/>
-      <c r="BY2" s="287"/>
-      <c r="BZ2" s="287"/>
-      <c r="CA2" s="287"/>
-      <c r="CB2" s="287"/>
-      <c r="CC2" s="287"/>
-      <c r="CD2" s="288"/>
-      <c r="CE2" s="286"/>
-      <c r="CF2" s="287"/>
-      <c r="CG2" s="287"/>
-      <c r="CH2" s="287"/>
-      <c r="CI2" s="287"/>
-      <c r="CJ2" s="287"/>
-      <c r="CK2" s="287"/>
-      <c r="CL2" s="287"/>
-      <c r="CM2" s="287"/>
-      <c r="CN2" s="288"/>
+      <c r="C2" s="283"/>
+      <c r="D2" s="284"/>
+      <c r="E2" s="284"/>
+      <c r="F2" s="284"/>
+      <c r="G2" s="284"/>
+      <c r="H2" s="284"/>
+      <c r="I2" s="284"/>
+      <c r="J2" s="284"/>
+      <c r="K2" s="284"/>
+      <c r="L2" s="284"/>
+      <c r="M2" s="284"/>
+      <c r="N2" s="284"/>
+      <c r="O2" s="284"/>
+      <c r="P2" s="284"/>
+      <c r="Q2" s="284"/>
+      <c r="R2" s="284"/>
+      <c r="S2" s="284"/>
+      <c r="T2" s="284"/>
+      <c r="U2" s="284"/>
+      <c r="V2" s="284"/>
+      <c r="W2" s="284"/>
+      <c r="X2" s="284"/>
+      <c r="Y2" s="284"/>
+      <c r="Z2" s="284"/>
+      <c r="AA2" s="284"/>
+      <c r="AB2" s="284"/>
+      <c r="AC2" s="284"/>
+      <c r="AD2" s="284"/>
+      <c r="AE2" s="284"/>
+      <c r="AF2" s="284"/>
+      <c r="AG2" s="284"/>
+      <c r="AH2" s="284"/>
+      <c r="AI2" s="284"/>
+      <c r="AJ2" s="284"/>
+      <c r="AK2" s="284"/>
+      <c r="AL2" s="284"/>
+      <c r="AM2" s="284"/>
+      <c r="AN2" s="284"/>
+      <c r="AO2" s="284"/>
+      <c r="AP2" s="284"/>
+      <c r="AQ2" s="284"/>
+      <c r="AR2" s="284"/>
+      <c r="AS2" s="284"/>
+      <c r="AT2" s="284"/>
+      <c r="AU2" s="284"/>
+      <c r="AV2" s="284"/>
+      <c r="AW2" s="284"/>
+      <c r="AX2" s="284"/>
+      <c r="AY2" s="284"/>
+      <c r="AZ2" s="284"/>
+      <c r="BA2" s="284"/>
+      <c r="BB2" s="284"/>
+      <c r="BC2" s="284"/>
+      <c r="BD2" s="284"/>
+      <c r="BE2" s="284"/>
+      <c r="BF2" s="284"/>
+      <c r="BG2" s="284"/>
+      <c r="BH2" s="284"/>
+      <c r="BI2" s="284"/>
+      <c r="BJ2" s="284"/>
+      <c r="BK2" s="284"/>
+      <c r="BL2" s="284"/>
+      <c r="BM2" s="284"/>
+      <c r="BN2" s="284"/>
+      <c r="BO2" s="284"/>
+      <c r="BP2" s="284"/>
+      <c r="BQ2" s="284"/>
+      <c r="BR2" s="284"/>
+      <c r="BS2" s="284"/>
+      <c r="BT2" s="284"/>
+      <c r="BU2" s="284"/>
+      <c r="BV2" s="284"/>
+      <c r="BW2" s="284"/>
+      <c r="BX2" s="284"/>
+      <c r="BY2" s="284"/>
+      <c r="BZ2" s="284"/>
+      <c r="CA2" s="284"/>
+      <c r="CB2" s="284"/>
+      <c r="CC2" s="284"/>
+      <c r="CD2" s="285"/>
+      <c r="CE2" s="283"/>
+      <c r="CF2" s="284"/>
+      <c r="CG2" s="284"/>
+      <c r="CH2" s="284"/>
+      <c r="CI2" s="284"/>
+      <c r="CJ2" s="284"/>
+      <c r="CK2" s="284"/>
+      <c r="CL2" s="284"/>
+      <c r="CM2" s="284"/>
+      <c r="CN2" s="285"/>
       <c r="CO2" s="103"/>
       <c r="CP2" s="139"/>
       <c r="CQ2" s="139"/>
@@ -17775,134 +17777,134 @@
       <c r="CV2" s="139"/>
     </row>
     <row r="3" spans="1:100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="290"/>
-      <c r="B3" s="292"/>
-      <c r="C3" s="280" t="s">
+      <c r="A3" s="287"/>
+      <c r="B3" s="289"/>
+      <c r="C3" s="291" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="281"/>
-      <c r="E3" s="281"/>
-      <c r="F3" s="281"/>
-      <c r="G3" s="282"/>
-      <c r="H3" s="280" t="s">
+      <c r="D3" s="292"/>
+      <c r="E3" s="292"/>
+      <c r="F3" s="292"/>
+      <c r="G3" s="293"/>
+      <c r="H3" s="291" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="281"/>
-      <c r="J3" s="281"/>
-      <c r="K3" s="281"/>
-      <c r="L3" s="282"/>
-      <c r="M3" s="280" t="s">
+      <c r="I3" s="292"/>
+      <c r="J3" s="292"/>
+      <c r="K3" s="292"/>
+      <c r="L3" s="293"/>
+      <c r="M3" s="291" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="281"/>
-      <c r="O3" s="281"/>
-      <c r="P3" s="281"/>
-      <c r="Q3" s="282"/>
-      <c r="R3" s="280" t="s">
+      <c r="N3" s="292"/>
+      <c r="O3" s="292"/>
+      <c r="P3" s="292"/>
+      <c r="Q3" s="293"/>
+      <c r="R3" s="291" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="281"/>
-      <c r="T3" s="281"/>
-      <c r="U3" s="281"/>
-      <c r="V3" s="282"/>
-      <c r="W3" s="280" t="s">
+      <c r="S3" s="292"/>
+      <c r="T3" s="292"/>
+      <c r="U3" s="292"/>
+      <c r="V3" s="293"/>
+      <c r="W3" s="291" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="281"/>
-      <c r="Y3" s="281"/>
-      <c r="Z3" s="281"/>
-      <c r="AA3" s="282"/>
-      <c r="AB3" s="280" t="s">
+      <c r="X3" s="292"/>
+      <c r="Y3" s="292"/>
+      <c r="Z3" s="292"/>
+      <c r="AA3" s="293"/>
+      <c r="AB3" s="291" t="s">
         <v>65</v>
       </c>
-      <c r="AC3" s="281"/>
-      <c r="AD3" s="281"/>
-      <c r="AE3" s="281"/>
-      <c r="AF3" s="282"/>
-      <c r="AG3" s="280" t="s">
+      <c r="AC3" s="292"/>
+      <c r="AD3" s="292"/>
+      <c r="AE3" s="292"/>
+      <c r="AF3" s="293"/>
+      <c r="AG3" s="291" t="s">
         <v>10</v>
       </c>
-      <c r="AH3" s="281"/>
-      <c r="AI3" s="281"/>
-      <c r="AJ3" s="281"/>
-      <c r="AK3" s="282"/>
-      <c r="AL3" s="280" t="s">
+      <c r="AH3" s="292"/>
+      <c r="AI3" s="292"/>
+      <c r="AJ3" s="292"/>
+      <c r="AK3" s="293"/>
+      <c r="AL3" s="291" t="s">
         <v>8</v>
       </c>
-      <c r="AM3" s="281"/>
-      <c r="AN3" s="281"/>
-      <c r="AO3" s="281"/>
-      <c r="AP3" s="282"/>
-      <c r="AQ3" s="280" t="s">
+      <c r="AM3" s="292"/>
+      <c r="AN3" s="292"/>
+      <c r="AO3" s="292"/>
+      <c r="AP3" s="293"/>
+      <c r="AQ3" s="291" t="s">
         <v>37</v>
       </c>
-      <c r="AR3" s="281"/>
-      <c r="AS3" s="281"/>
-      <c r="AT3" s="281"/>
-      <c r="AU3" s="282"/>
-      <c r="AV3" s="280" t="s">
+      <c r="AR3" s="292"/>
+      <c r="AS3" s="292"/>
+      <c r="AT3" s="292"/>
+      <c r="AU3" s="293"/>
+      <c r="AV3" s="291" t="s">
         <v>80</v>
       </c>
-      <c r="AW3" s="281"/>
-      <c r="AX3" s="281"/>
-      <c r="AY3" s="281"/>
-      <c r="AZ3" s="282"/>
-      <c r="BA3" s="280" t="s">
+      <c r="AW3" s="292"/>
+      <c r="AX3" s="292"/>
+      <c r="AY3" s="292"/>
+      <c r="AZ3" s="293"/>
+      <c r="BA3" s="291" t="s">
         <v>81</v>
       </c>
-      <c r="BB3" s="281"/>
-      <c r="BC3" s="281"/>
-      <c r="BD3" s="281"/>
-      <c r="BE3" s="282"/>
-      <c r="BF3" s="280" t="s">
+      <c r="BB3" s="292"/>
+      <c r="BC3" s="292"/>
+      <c r="BD3" s="292"/>
+      <c r="BE3" s="293"/>
+      <c r="BF3" s="291" t="s">
         <v>82</v>
       </c>
-      <c r="BG3" s="281"/>
-      <c r="BH3" s="281"/>
-      <c r="BI3" s="281"/>
-      <c r="BJ3" s="282"/>
-      <c r="BK3" s="280" t="s">
+      <c r="BG3" s="292"/>
+      <c r="BH3" s="292"/>
+      <c r="BI3" s="292"/>
+      <c r="BJ3" s="293"/>
+      <c r="BK3" s="291" t="s">
         <v>79</v>
       </c>
-      <c r="BL3" s="281"/>
-      <c r="BM3" s="281"/>
-      <c r="BN3" s="281"/>
-      <c r="BO3" s="282"/>
-      <c r="BP3" s="280" t="s">
+      <c r="BL3" s="292"/>
+      <c r="BM3" s="292"/>
+      <c r="BN3" s="292"/>
+      <c r="BO3" s="293"/>
+      <c r="BP3" s="291" t="s">
         <v>83</v>
       </c>
-      <c r="BQ3" s="281"/>
-      <c r="BR3" s="281"/>
-      <c r="BS3" s="281"/>
-      <c r="BT3" s="282"/>
-      <c r="BU3" s="280" t="s">
+      <c r="BQ3" s="292"/>
+      <c r="BR3" s="292"/>
+      <c r="BS3" s="292"/>
+      <c r="BT3" s="293"/>
+      <c r="BU3" s="291" t="s">
         <v>84</v>
       </c>
-      <c r="BV3" s="281"/>
-      <c r="BW3" s="281"/>
-      <c r="BX3" s="281"/>
-      <c r="BY3" s="282"/>
-      <c r="BZ3" s="280" t="s">
+      <c r="BV3" s="292"/>
+      <c r="BW3" s="292"/>
+      <c r="BX3" s="292"/>
+      <c r="BY3" s="293"/>
+      <c r="BZ3" s="291" t="s">
         <v>66</v>
       </c>
-      <c r="CA3" s="281"/>
-      <c r="CB3" s="281"/>
-      <c r="CC3" s="281"/>
-      <c r="CD3" s="282"/>
-      <c r="CE3" s="280" t="s">
+      <c r="CA3" s="292"/>
+      <c r="CB3" s="292"/>
+      <c r="CC3" s="292"/>
+      <c r="CD3" s="293"/>
+      <c r="CE3" s="291" t="s">
         <v>76</v>
       </c>
-      <c r="CF3" s="281"/>
-      <c r="CG3" s="281"/>
-      <c r="CH3" s="281"/>
-      <c r="CI3" s="282"/>
-      <c r="CJ3" s="280" t="s">
+      <c r="CF3" s="292"/>
+      <c r="CG3" s="292"/>
+      <c r="CH3" s="292"/>
+      <c r="CI3" s="293"/>
+      <c r="CJ3" s="291" t="s">
         <v>75</v>
       </c>
-      <c r="CK3" s="281"/>
-      <c r="CL3" s="281"/>
-      <c r="CM3" s="281"/>
-      <c r="CN3" s="282"/>
+      <c r="CK3" s="292"/>
+      <c r="CL3" s="292"/>
+      <c r="CM3" s="292"/>
+      <c r="CN3" s="293"/>
       <c r="CO3" s="103"/>
       <c r="CP3" s="139"/>
       <c r="CQ3" s="139"/>
@@ -17913,8 +17915,8 @@
       <c r="CV3" s="139"/>
     </row>
     <row r="4" spans="1:100" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="290"/>
-      <c r="B4" s="293"/>
+      <c r="A4" s="287"/>
+      <c r="B4" s="290"/>
       <c r="C4" s="175">
         <v>5</v>
       </c>
@@ -18195,10 +18197,10 @@
       <c r="CV4" s="139"/>
     </row>
     <row r="5" spans="1:100" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="285" t="s">
+      <c r="A5" s="282" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="284">
+      <c r="B5" s="281">
         <f>УРС!AB3+УРС!AC3</f>
         <v>0</v>
       </c>
@@ -18571,8 +18573,8 @@
       <c r="CV5" s="139"/>
     </row>
     <row r="6" spans="1:100" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="285"/>
-      <c r="B6" s="284"/>
+      <c r="A6" s="282"/>
+      <c r="B6" s="281"/>
       <c r="C6" s="181">
         <f>IF(ISERR(C5/SUM(C5:F5)*100),0,C5/SUM(C5:F5)*100)</f>
         <v>0</v>
@@ -19139,14 +19141,14 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <customSheetViews>
-    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" scale="70" showPageBreaks="1" fitToPage="1" printArea="1" hiddenRows="1" view="pageBreakPreview">
+    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" scale="70" showPageBreaks="1" fitToPage="1" printArea="1" hiddenRows="1" view="pageBreakPreview">
       <selection activeCell="AB158" sqref="AB158"/>
       <pageMargins left="0.5" right="0.25" top="0.64" bottom="0.19685039370078741" header="0.25" footer="0.34"/>
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="57" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" scale="70" showPageBreaks="1" fitToPage="1" printArea="1" hiddenRows="1" view="pageBreakPreview">
+    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" scale="70" showPageBreaks="1" fitToPage="1" printArea="1" hiddenRows="1" view="pageBreakPreview">
       <selection activeCell="AB158" sqref="AB158"/>
       <pageMargins left="0.5" right="0.25" top="0.64" bottom="0.19685039370078741" header="0.25" footer="0.34"/>
       <printOptions horizontalCentered="1"/>
@@ -19155,6 +19157,15 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="25">
+    <mergeCell ref="BF3:BJ3"/>
+    <mergeCell ref="BK3:BO3"/>
+    <mergeCell ref="BP3:BT3"/>
+    <mergeCell ref="BU3:BY3"/>
+    <mergeCell ref="AB3:AF3"/>
+    <mergeCell ref="AG3:AK3"/>
+    <mergeCell ref="AL3:AP3"/>
+    <mergeCell ref="AV3:AZ3"/>
+    <mergeCell ref="BA3:BE3"/>
     <mergeCell ref="A1:CN1"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
@@ -19171,15 +19182,6 @@
     <mergeCell ref="BZ3:CD3"/>
     <mergeCell ref="R3:V3"/>
     <mergeCell ref="W3:AA3"/>
-    <mergeCell ref="BF3:BJ3"/>
-    <mergeCell ref="BK3:BO3"/>
-    <mergeCell ref="BP3:BT3"/>
-    <mergeCell ref="BU3:BY3"/>
-    <mergeCell ref="AB3:AF3"/>
-    <mergeCell ref="AG3:AK3"/>
-    <mergeCell ref="AL3:AP3"/>
-    <mergeCell ref="AV3:AZ3"/>
-    <mergeCell ref="BA3:BE3"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -37292,13 +37294,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" hiddenColumns="1" state="hidden" topLeftCell="A39">
+    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" hiddenColumns="1" state="hidden" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
+    <customSheetView guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId2"/>
@@ -37310,13 +37312,13 @@
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{098CBCA2-BBCD-46DE-A03A-A0F02BA0B003}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
+    <customSheetView guid="{177FEA91-3CC1-47AE-B40C-764C2A914D34}" hiddenColumns="1" state="hidden" showRuler="0" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId4"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{9C80F5BB-2041-4866-B668-5D20F7DCF520}" hiddenColumns="1" state="hidden" topLeftCell="A39">
+    <customSheetView guid="{02FA8FE8-A21A-4BA6-9778-A92892052DF2}" hiddenColumns="1" state="hidden" topLeftCell="A39">
       <selection activeCell="R52" sqref="R52"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId5"/>

</xml_diff>